<commit_message>
added logger, constants, fixed parsing header
</commit_message>
<xml_diff>
--- a/accept-excel/accept-excel-svc/testFiles/excelTest.xlsx
+++ b/accept-excel/accept-excel-svc/testFiles/excelTest.xlsx
@@ -4,12 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="132" windowWidth="22932" windowHeight="9240"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="12012" windowHeight="4788"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -18,18 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
-    <t>Sno.</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
     <t>PY</t>
   </si>
   <si>
@@ -46,6 +32,18 @@
   </si>
   <si>
     <t>LS</t>
+  </si>
+  <si>
+    <t>Sno. [NUMERIC]</t>
+  </si>
+  <si>
+    <t>Name [STRING]</t>
+  </si>
+  <si>
+    <t>age [NUMERIC]</t>
+  </si>
+  <si>
+    <t>sex [STRING]</t>
   </si>
 </sst>
 </file>
@@ -380,23 +378,23 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -404,13 +402,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -418,13 +416,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -432,13 +430,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -446,40 +444,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
captured unparseable to a list & improved regex
</commit_message>
<xml_diff>
--- a/accept-excel/accept-excel-svc/testFiles/excelTest.xlsx
+++ b/accept-excel/accept-excel-svc/testFiles/excelTest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>PY</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>sex [STRING]</t>
+  </si>
+  <si>
+    <t>prakhar yadav</t>
+  </si>
+  <si>
+    <t>2Six</t>
   </si>
 </sst>
 </file>
@@ -375,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -421,8 +427,8 @@
       <c r="C3">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -446,10 +452,24 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>26</v>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>